<commit_message>
realizacion de los calculos para potencia ideal
</commit_message>
<xml_diff>
--- a/Especificaciones - Copia.xlsx
+++ b/Especificaciones - Copia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rotorbike.sharepoint.com/sites/ROTORRD/Shared Documents/Power meters general/Software/Simulador/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal KEVIN\TRABAJOS DE CLASE PARA PORTAFOLIO\Simulador\PowerSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B2F716B-C0DF-4040-8334-1A84384F2B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C11A74-1BF5-42B8-878D-CD6C7CB7B87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada de datos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -240,12 +240,15 @@
   <si>
     <t>La parte referente a la velocidad angular está aún por definir.</t>
   </si>
+  <si>
+    <t>*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,20 +657,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="79.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="73.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="79.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="73.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -681,7 +684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>10</v>
       </c>
@@ -691,7 +694,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="60">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>20</v>
       </c>
@@ -701,7 +704,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>30</v>
       </c>
@@ -711,7 +714,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="105">
+    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>40</v>
       </c>
@@ -721,7 +724,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>50</v>
       </c>
@@ -731,7 +734,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>60</v>
       </c>
@@ -754,16 +757,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="79.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="73.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="79.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="73.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -777,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="216.75" customHeight="1">
+    <row r="2" spans="1:4" ht="216.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1010</v>
       </c>
@@ -787,7 +790,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1020</v>
       </c>
@@ -797,7 +800,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1030</v>
       </c>
@@ -807,7 +810,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1040</v>
       </c>
@@ -817,7 +820,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1050</v>
       </c>
@@ -827,17 +830,17 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -856,16 +859,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="79.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="73.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="79.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="73.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -879,7 +882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>2010</v>
       </c>
@@ -889,7 +892,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2020</v>
       </c>
@@ -899,7 +902,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2030</v>
       </c>
@@ -909,12 +912,12 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
@@ -928,20 +931,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6637741-2958-46F6-878E-148769F8164A}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="B10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="79.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="73.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="79.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="73.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -955,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>3010</v>
       </c>
@@ -965,27 +968,31 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="105">
+    <row r="3" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>3020</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="75">
+    <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3030</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3040</v>
       </c>
@@ -995,7 +1002,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="135">
+    <row r="6" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3050</v>
       </c>
@@ -1005,7 +1012,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="75">
+    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>3060</v>
       </c>
@@ -1015,7 +1022,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>3070</v>
       </c>
@@ -1025,7 +1032,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="90">
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>3080</v>
       </c>
@@ -1035,7 +1042,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="135">
+    <row r="10" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3090</v>
       </c>
@@ -1054,20 +1061,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3BE08-B24D-4818-921F-0F619E53D40A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="79.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="73.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="79.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="73.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>3010</v>
       </c>
@@ -1091,7 +1098,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="60">
+    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>3020</v>
       </c>
@@ -1101,7 +1108,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="120">
+    <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3030</v>
       </c>
@@ -1111,7 +1118,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3040</v>
       </c>
@@ -1121,7 +1128,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3050</v>
       </c>
@@ -1131,7 +1138,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="150">
+    <row r="7" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>3060</v>
       </c>
@@ -1141,7 +1148,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="75">
+    <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>3070</v>
       </c>
@@ -1151,7 +1158,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="60">
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>3080</v>
       </c>
@@ -1161,7 +1168,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3090</v>
       </c>
@@ -1171,7 +1178,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="150">
+    <row r="11" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>3090</v>
       </c>
@@ -1181,7 +1188,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="45">
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>3100</v>
       </c>
@@ -1204,9 +1211,9 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1217,14 +1224,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef609709-056e-4bd4-acdb-309fc487b936">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="36f9d292-2d4b-45a6-8703-2a8b9ed34337" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1483,22 +1488,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef609709-056e-4bd4-acdb-309fc487b936">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="36f9d292-2d4b-45a6-8703-2a8b9ed34337" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef609709-056e-4bd4-acdb-309fc487b936"/>
+    <ds:schemaRef ds:uri="36f9d292-2d4b-45a6-8703-2a8b9ed34337"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef609709-056e-4bd4-acdb-309fc487b936"/>
+    <ds:schemaRef ds:uri="36f9d292-2d4b-45a6-8703-2a8b9ed34337"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado suma de todos los sectores al terminar los resultados de potencia por sectores
</commit_message>
<xml_diff>
--- a/Especificaciones - Copia.xlsx
+++ b/Especificaciones - Copia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal KEVIN\TRABAJOS DE CLASE PARA PORTAFOLIO\Simulador\PowerSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C11A74-1BF5-42B8-878D-CD6C7CB7B87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19168D9F-9947-47DE-B1CC-C59619DBEE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada de datos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Listo</t>
   </si>
 </sst>
 </file>
@@ -931,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6637741-2958-46F6-878E-148769F8164A}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1061,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3BE08-B24D-4818-921F-0F619E53D40A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1098,9 @@
       <c r="B2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -1105,7 +1110,9 @@
       <c r="B3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -1115,7 +1122,9 @@
       <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -1125,7 +1134,9 @@
       <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1135,7 +1146,9 @@
       <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
@@ -1233,6 +1246,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef609709-056e-4bd4-acdb-309fc487b936">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="36f9d292-2d4b-45a6-8703-2a8b9ed34337" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010034CD6C630D9F0C499835E219551B69CE" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="030c5622b615cff52946ce70866134ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef609709-056e-4bd4-acdb-309fc487b936" xmlns:ns3="36f9d292-2d4b-45a6-8703-2a8b9ed34337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128154f498505afae3420639940d45d6" ns2:_="" ns3:_="">
     <xsd:import namespace="ef609709-056e-4bd4-acdb-309fc487b936"/>
@@ -1487,17 +1511,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef609709-056e-4bd4-acdb-309fc487b936">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="36f9d292-2d4b-45a6-8703-2a8b9ed34337" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
   <ds:schemaRefs>
@@ -1507,6 +1520,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef609709-056e-4bd4-acdb-309fc487b936"/>
+    <ds:schemaRef ds:uri="36f9d292-2d4b-45a6-8703-2a8b9ed34337"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1523,15 +1547,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef609709-056e-4bd4-acdb-309fc487b936"/>
-    <ds:schemaRef ds:uri="36f9d292-2d4b-45a6-8703-2a8b9ed34337"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado balance de error por sectores en pestaña calculos por sectores pero algo en los resultados no parece estar bien
</commit_message>
<xml_diff>
--- a/Especificaciones - Copia.xlsx
+++ b/Especificaciones - Copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal KEVIN\TRABAJOS DE CLASE PARA PORTAFOLIO\Simulador\PowerSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19168D9F-9947-47DE-B1CC-C59619DBEE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA867A-B048-4AF5-9531-12BDAE6EF7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>Listo</t>
+  </si>
+  <si>
+    <t>falta</t>
+  </si>
+  <si>
+    <t>algo falla</t>
+  </si>
+  <si>
+    <t>Los valores de izquierda son muy altos en el balance…</t>
+  </si>
+  <si>
+    <t>Trabajando en ello</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3BE08-B24D-4818-921F-0F619E53D40A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,7 +1170,9 @@
       <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -1168,7 +1182,9 @@
       <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -1178,7 +1194,9 @@
       <c r="B9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1188,8 +1206,12 @@
       <c r="B10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
@@ -1198,7 +1220,9 @@
       <c r="B11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1213,6 +1237,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1246,17 +1271,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef609709-056e-4bd4-acdb-309fc487b936">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="36f9d292-2d4b-45a6-8703-2a8b9ed34337" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010034CD6C630D9F0C499835E219551B69CE" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="030c5622b615cff52946ce70866134ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef609709-056e-4bd4-acdb-309fc487b936" xmlns:ns3="36f9d292-2d4b-45a6-8703-2a8b9ed34337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128154f498505afae3420639940d45d6" ns2:_="" ns3:_="">
     <xsd:import namespace="ef609709-056e-4bd4-acdb-309fc487b936"/>
@@ -1511,6 +1525,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef609709-056e-4bd4-acdb-309fc487b936">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="36f9d292-2d4b-45a6-8703-2a8b9ed34337" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
   <ds:schemaRefs>
@@ -1520,17 +1545,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef609709-056e-4bd4-acdb-309fc487b936"/>
-    <ds:schemaRef ds:uri="36f9d292-2d4b-45a6-8703-2a8b9ed34337"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1547,4 +1561,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef609709-056e-4bd4-acdb-309fc487b936"/>
+    <ds:schemaRef ds:uri="36f9d292-2d4b-45a6-8703-2a8b9ed34337"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
botones y graficas para sectores colocados
</commit_message>
<xml_diff>
--- a/Especificaciones - Copia.xlsx
+++ b/Especificaciones - Copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal KEVIN\TRABAJOS DE CLASE PARA PORTAFOLIO\Simulador\PowerSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA867A-B048-4AF5-9531-12BDAE6EF7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA0720-0034-4CE9-B224-6D7E47D34353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1076,15 +1076,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3BE08-B24D-4818-921F-0F619E53D40A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="79.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="73.44140625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
@@ -1262,15 +1262,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010034CD6C630D9F0C499835E219551B69CE" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="030c5622b615cff52946ce70866134ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef609709-056e-4bd4-acdb-309fc487b936" xmlns:ns3="36f9d292-2d4b-45a6-8703-2a8b9ed34337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128154f498505afae3420639940d45d6" ns2:_="" ns3:_="">
     <xsd:import namespace="ef609709-056e-4bd4-acdb-309fc487b936"/>
@@ -1525,6 +1516,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1537,14 +1537,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1563,6 +1555,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
documentando codigo y puesta en marcha la grafia, verificar las indicaciones para ver las dudas que tengo y con lo que basicamente ya estaria todo este apartado
</commit_message>
<xml_diff>
--- a/Especificaciones - Copia.xlsx
+++ b/Especificaciones - Copia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal KEVIN\TRABAJOS DE CLASE PARA PORTAFOLIO\Simulador\PowerSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA0720-0034-4CE9-B224-6D7E47D34353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940F1789-B789-4A7F-8C0E-EA5673A9ADD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada de datos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -256,7 +256,16 @@
     <t>Los valores de izquierda son muy altos en el balance…</t>
   </si>
   <si>
-    <t>Trabajando en ello</t>
+    <t>ERROR DE POTENCIA? Para eso seria necesario una potencia ideal, según la formula que tengo.</t>
+  </si>
+  <si>
+    <t>casi terminado</t>
+  </si>
+  <si>
+    <t>El balance de error de los sectores y el resultado de los calculos son algo altos…</t>
+  </si>
+  <si>
+    <t>Creo que algo falla.</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3BE08-B24D-4818-921F-0F619E53D40A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,9 +1204,11 @@
         <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
@@ -1221,9 +1232,11 @@
         <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
@@ -1262,6 +1275,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010034CD6C630D9F0C499835E219551B69CE" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="030c5622b615cff52946ce70866134ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef609709-056e-4bd4-acdb-309fc487b936" xmlns:ns3="36f9d292-2d4b-45a6-8703-2a8b9ed34337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128154f498505afae3420639940d45d6" ns2:_="" ns3:_="">
     <xsd:import namespace="ef609709-056e-4bd4-acdb-309fc487b936"/>
@@ -1516,15 +1538,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1537,6 +1550,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1555,14 +1576,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
prueba con la multigrafica, no se dibuja bien
</commit_message>
<xml_diff>
--- a/Especificaciones - Copia.xlsx
+++ b/Especificaciones - Copia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal KEVIN\TRABAJOS DE CLASE PARA PORTAFOLIO\Simulador\PowerSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940F1789-B789-4A7F-8C0E-EA5673A9ADD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865723CE-0E0F-4DB1-ABE4-54F598153A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33675" yWindow="2595" windowWidth="17280" windowHeight="8970" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada de datos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -250,9 +250,6 @@
     <t>falta</t>
   </si>
   <si>
-    <t>algo falla</t>
-  </si>
-  <si>
     <t>Los valores de izquierda son muy altos en el balance…</t>
   </si>
   <si>
@@ -265,7 +262,7 @@
     <t>El balance de error de los sectores y el resultado de los calculos son algo altos…</t>
   </si>
   <si>
-    <t>Creo que algo falla.</t>
+    <t>listo</t>
   </si>
 </sst>
 </file>
@@ -1085,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3BE08-B24D-4818-921F-0F619E53D40A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,10 +1201,10 @@
         <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1218,10 +1215,10 @@
         <v>39</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="144" x14ac:dyDescent="0.3">
@@ -1232,10 +1229,10 @@
         <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1275,15 +1272,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010034CD6C630D9F0C499835E219551B69CE" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="030c5622b615cff52946ce70866134ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef609709-056e-4bd4-acdb-309fc487b936" xmlns:ns3="36f9d292-2d4b-45a6-8703-2a8b9ed34337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128154f498505afae3420639940d45d6" ns2:_="" ns3:_="">
     <xsd:import namespace="ef609709-056e-4bd4-acdb-309fc487b936"/>
@@ -1538,6 +1526,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1550,14 +1547,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03AB5BBB-C11C-49C0-856A-B316563A29AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1576,6 +1565,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B811C3F4-06FB-4D14-867C-E45A3249AFA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87C67367-DAA4-4EB3-B534-41A7BE44AD0D}">
   <ds:schemaRefs>

</xml_diff>